<commit_message>
Bug fixed: multishooting on same field
ToDO: optimize gameLoop()
</commit_message>
<xml_diff>
--- a/C++/TDD.xlsx
+++ b/C++/TDD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>X</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>- Gesperrter Bereich mein Setzen schreibt über grenze</t>
+  </si>
+  <si>
+    <t>- beim drehen auf andere Schiffe konrollieren</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +87,11 @@
       <patternFill patternType="gray125">
         <fgColor rgb="FFFF0000"/>
         <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -234,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,6 +285,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,7 +589,7 @@
   <dimension ref="P3:AC34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.28515625" defaultRowHeight="15"/>
@@ -666,9 +680,15 @@
         <v>1</v>
       </c>
       <c r="Q9" s="5"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
+      <c r="R9" s="6">
+        <v>3</v>
+      </c>
+      <c r="S9" s="6">
+        <v>3</v>
+      </c>
+      <c r="T9" s="6">
+        <v>3</v>
+      </c>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
@@ -682,9 +702,15 @@
         <v>2</v>
       </c>
       <c r="Q10" s="5"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
+      <c r="R10" s="6">
+        <v>3</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="T10" s="6">
+        <v>3</v>
+      </c>
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
@@ -698,8 +724,12 @@
         <v>3</v>
       </c>
       <c r="Q11" s="5"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
+      <c r="R11" s="6">
+        <v>3</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="T11" s="6">
         <v>3</v>
       </c>
@@ -720,8 +750,12 @@
         <v>4</v>
       </c>
       <c r="Q12" s="5"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
+      <c r="R12" s="6">
+        <v>3</v>
+      </c>
+      <c r="S12" s="6">
+        <v>3</v>
+      </c>
       <c r="T12" s="6">
         <v>3</v>
       </c>
@@ -769,8 +803,8 @@
       <c r="T14" s="6">
         <v>3</v>
       </c>
-      <c r="U14" s="6">
-        <v>3</v>
+      <c r="U14" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="V14" s="6">
         <v>3</v>
@@ -788,9 +822,15 @@
       <c r="Q15" s="5"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
+      <c r="T15" s="15">
+        <v>3</v>
+      </c>
+      <c r="U15" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" s="15">
+        <v>3</v>
+      </c>
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
       <c r="Y15" s="7"/>
@@ -804,9 +844,15 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
+      <c r="T16" s="15">
+        <v>3</v>
+      </c>
+      <c r="U16" s="15">
+        <v>3</v>
+      </c>
+      <c r="V16" s="15">
+        <v>3</v>
+      </c>
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
       <c r="Y16" s="7"/>
@@ -858,7 +904,7 @@
     </row>
     <row r="23" spans="16:27">
       <c r="P23" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="16:27">
@@ -882,7 +928,9 @@
       </c>
     </row>
     <row r="29" spans="16:27">
-      <c r="P29" s="13"/>
+      <c r="P29" s="14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="16:27">
       <c r="P30" s="13"/>

</xml_diff>